<commit_message>
#153 & #167 medium completed.
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Work/Git/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34779FEB-41E6-2745-81DE-42E549034F9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E89E0F9-59E1-954C-8BFA-066C97D148B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{00BFEBED-41FD-4445-A067-D74A6DA3447C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Title</t>
   </si>
@@ -105,6 +105,27 @@
   </si>
   <si>
     <t>Iterate over the list maintaining the min and max vales between the number itself and its products with min and max. Return the greatest max.</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>O(log n)</t>
+  </si>
+  <si>
+    <t>Binary search keeping in mind the rotation point in the array. Determine if the middle is part of the "left" or "right" side of the array.</t>
+  </si>
+  <si>
+    <t>Two Sum II - Input Array Is Sorted</t>
+  </si>
+  <si>
+    <t>Array, Two iters</t>
+  </si>
+  <si>
+    <t>Same idea as a binary search with no middle. Move the right and left iters in increments of 1 based on if the sum of those iters is less or greater than the target.</t>
   </si>
 </sst>
 </file>
@@ -520,16 +541,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F48452-0640-744E-B61C-1E2914A6E373}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="149.1640625" customWidth="1"/>
@@ -675,6 +696,46 @@
         <v>23</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>152</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>167</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Binary search / Brute-Force search comparison.
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Work/Git/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2FE2AF-1E19-F040-AA9B-64DA61ECA576}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51638937-0703-EA44-BB9B-6B9560F40E4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{00BFEBED-41FD-4445-A067-D74A6DA3447C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Title</t>
   </si>
@@ -147,13 +147,19 @@
   </si>
   <si>
     <t>Push all the values to a stack and modify them based on the given operations.</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>Only works on sorted arrays. Sliding window across entire array, calculating the middle between the left/right iters. Move left/right iter based on the middle value.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,8 +197,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +220,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
       </patternFill>
     </fill>
   </fills>
@@ -228,13 +246,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -245,8 +264,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Extra" xfId="4" xr:uid="{37FE978E-75C6-F943-AD7D-18755893BBB0}"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
@@ -562,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F48452-0640-744E-B61C-1E2914A6E373}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -797,6 +818,23 @@
         <v>37</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>